<commit_message>
commited without staging 1 file
</commit_message>
<xml_diff>
--- a/xyz.xlsx
+++ b/xyz.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>acck</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>akdcj</t>
+  </si>
+  <si>
+    <t>sdc</t>
   </si>
 </sst>
 </file>
@@ -369,7 +372,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -382,6 +385,11 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G10" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>